<commit_message>
Topology-SOSA/SSN adapter diagram (ontologyt not yet updated)
</commit_message>
<xml_diff>
--- a/Source_data/IFC/Embankment sample file, Davide Pifferi/4x3_IFC_RI02-sfa.xlsx
+++ b/Source_data/IFC/Embankment sample file, Davide Pifferi/4x3_IFC_RI02-sfa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PycharmProjects\SemanticRSM\Source_data\IFC\Embankment sample file, Davide Pifferi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F4ED1D87-1865-4684-8C16-1FF7D20631A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D0C4F0-71E1-4AB2-B8FA-13EC095D48D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="43396" windowHeight="23776" tabRatio="700" firstSheet="25" activeTab="37" xr2:uid="{17A6E86C-1C29-425E-9B1D-0C3B966F99B8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="43396" windowHeight="23776" tabRatio="700" xr2:uid="{17A6E86C-1C29-425E-9B1D-0C3B966F99B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="42" r:id="rId1"/>
@@ -11409,9 +11409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A38E87-3658-4500-B432-C4A537444EE6}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12127,7 +12127,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -20462,7 +20462,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:C1"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -40753,7 +40753,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:G1"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -48646,7 +48646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61021095-0324-4C3F-AB2F-144CFFD24C38}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>